<commit_message>
cleaned up data in trace elements plot
</commit_message>
<xml_diff>
--- a/data/geochemistry/trace_elements_plots.xlsx
+++ b/data/geochemistry/trace_elements_plots.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/staceygerasimov/0000_Spring_2022/Berkeley Hills Manucript/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/staceygerasimov/0000_Spring_2022/0000_Github/Gerasimov_Berkeley_Hills/data/geochemistry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F179A840-B7FE-2640-8C79-0392125F59E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C518B9E-D3DF-ED48-961D-0B08FD12D2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="26020" windowHeight="16460" xr2:uid="{B4E318BD-809D-B847-842E-474829749670}"/>
   </bookViews>
@@ -182,10 +182,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -5764,52 +5763,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>185718</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>22581</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>660018</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>161190</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0488A845-6514-C343-985A-032F55480816}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:alphaModFix amt="53000"/>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19402823" y="1827318"/>
-          <a:ext cx="10500616" cy="9964398"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6204,21 +6157,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -6237,7 +6190,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -6256,7 +6209,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -6275,7 +6228,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6">
@@ -6294,7 +6247,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7">
@@ -6313,7 +6266,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8">
@@ -6332,7 +6285,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B9">
@@ -6351,7 +6304,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B10">
@@ -6370,7 +6323,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B11">
@@ -6389,7 +6342,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B12">
@@ -6408,7 +6361,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13">
@@ -6427,7 +6380,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14">
@@ -6446,7 +6399,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B15">
@@ -6465,7 +6418,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B16">
@@ -6484,7 +6437,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17">
@@ -6503,7 +6456,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18">
@@ -6522,7 +6475,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B19">
@@ -6541,7 +6494,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B20">
@@ -6560,7 +6513,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B21">
@@ -6579,7 +6532,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B22">
@@ -6598,7 +6551,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23">
@@ -6617,7 +6570,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B24">
@@ -6636,7 +6589,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B25">
@@ -6655,7 +6608,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B26">
@@ -6674,7 +6627,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B27">
@@ -6693,7 +6646,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B28">
@@ -6712,7 +6665,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B29">
@@ -6731,7 +6684,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B30">
@@ -6750,7 +6703,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B31">
@@ -6769,7 +6722,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B32">
@@ -6788,7 +6741,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B33">
@@ -6807,7 +6760,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B34">
@@ -6826,7 +6779,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B35">
@@ -6845,7 +6798,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B36">
@@ -6864,7 +6817,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B37">
@@ -6883,7 +6836,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B38">
@@ -6902,7 +6855,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B39">
@@ -6921,7 +6874,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B40">
@@ -6940,7 +6893,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B41">
@@ -6959,7 +6912,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B42">
@@ -6978,7 +6931,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B43">
@@ -6997,7 +6950,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B44">
@@ -7016,7 +6969,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B45">
@@ -7035,7 +6988,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B46">
@@ -7054,7 +7007,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B47">
@@ -7073,7 +7026,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B48">
@@ -7092,7 +7045,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B49">
@@ -7111,7 +7064,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B50">
@@ -7130,7 +7083,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B51">
@@ -7149,7 +7102,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B52">
@@ -7168,7 +7121,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B53">
@@ -7187,7 +7140,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B54">
@@ -7206,7 +7159,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B55">
@@ -7225,7 +7178,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B56">
@@ -7244,7 +7197,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B57">
@@ -7263,7 +7216,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B58">
@@ -7282,7 +7235,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B59">
@@ -7301,7 +7254,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B60">
@@ -7320,7 +7273,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B61">
@@ -7339,7 +7292,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B62">
@@ -7358,7 +7311,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B63">
@@ -7377,7 +7330,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B64">
@@ -7396,7 +7349,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B65">
@@ -7415,7 +7368,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B66">
@@ -7434,7 +7387,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B67">
@@ -7453,7 +7406,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B68">
@@ -7472,7 +7425,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B69">
@@ -7491,7 +7444,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B70">
@@ -7510,7 +7463,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B71">
@@ -7529,7 +7482,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B72">
@@ -7548,7 +7501,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B73">
@@ -7567,7 +7520,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B74">
@@ -7586,7 +7539,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B75">
@@ -7605,7 +7558,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B76">
@@ -7624,7 +7577,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B77">
@@ -7643,7 +7596,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B78">
@@ -7662,7 +7615,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B79">
@@ -7681,7 +7634,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B80">
@@ -7700,7 +7653,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B81">
@@ -7719,7 +7672,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B82">
@@ -7738,7 +7691,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B83">
@@ -7757,7 +7710,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B84">
@@ -7776,7 +7729,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B85">
@@ -7795,7 +7748,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B86">
@@ -7814,7 +7767,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B87">
@@ -7833,7 +7786,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B88">
@@ -7852,7 +7805,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B89">
@@ -7871,7 +7824,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B90">
@@ -7890,7 +7843,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B91">
@@ -7909,7 +7862,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B92">
@@ -7928,7 +7881,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B93">
@@ -7947,7 +7900,7 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B94">
@@ -7966,7 +7919,7 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B95">
@@ -7985,7 +7938,7 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B96">
@@ -8004,7 +7957,7 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B97">
@@ -8023,7 +7976,7 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B98">
@@ -8042,7 +7995,7 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B99">
@@ -8061,7 +8014,7 @@
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B100">
@@ -8080,7 +8033,7 @@
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B101">
@@ -8099,7 +8052,7 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B102">
@@ -8118,7 +8071,7 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B103">
@@ -8137,7 +8090,7 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B104">
@@ -8156,7 +8109,7 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B105">
@@ -8174,11 +8127,8 @@
         <v>-0.19594908907233738</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="2"/>
-    </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B107">
@@ -8197,7 +8147,7 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B108">
@@ -8216,7 +8166,7 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B109">
@@ -8235,7 +8185,7 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B110">
@@ -8254,7 +8204,7 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B111">
@@ -8273,7 +8223,7 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B112">
@@ -8292,7 +8242,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B113">
@@ -8311,7 +8261,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B114">
@@ -8330,7 +8280,7 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B115">
@@ -8349,7 +8299,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B116">
@@ -8368,7 +8318,7 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B117">
@@ -8387,7 +8337,7 @@
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B118">
@@ -8406,7 +8356,7 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B119">
@@ -8425,7 +8375,7 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B120">
@@ -8444,7 +8394,7 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B121">
@@ -8463,7 +8413,7 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B122">
@@ -8482,7 +8432,7 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B123">
@@ -8501,7 +8451,7 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B124">
@@ -8520,7 +8470,7 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B125">
@@ -8539,7 +8489,7 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B126">
@@ -8558,7 +8508,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B127">
@@ -8577,7 +8527,7 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B128">
@@ -8596,7 +8546,7 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B129">
@@ -8615,7 +8565,7 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B130">
@@ -8634,7 +8584,7 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B131">
@@ -8653,7 +8603,7 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B132">
@@ -8672,7 +8622,7 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B133">
@@ -8691,7 +8641,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
+      <c r="A134" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B134">
@@ -8710,7 +8660,7 @@
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
+      <c r="A135" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B135">
@@ -8729,7 +8679,7 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
+      <c r="A136" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B136">
@@ -8748,7 +8698,7 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
+      <c r="A137" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B137">
@@ -8767,7 +8717,7 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B138">
@@ -8786,7 +8736,7 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B139">
@@ -8805,7 +8755,7 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B140">
@@ -8824,7 +8774,7 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B141">
@@ -8843,7 +8793,7 @@
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B142">
@@ -8862,7 +8812,7 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B143">
@@ -8881,7 +8831,7 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B144">
@@ -8900,7 +8850,7 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
+      <c r="A145" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B145">
@@ -8919,7 +8869,7 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="4" t="s">
+      <c r="A146" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B146">
@@ -8938,7 +8888,7 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
+      <c r="A147" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B147">
@@ -8957,7 +8907,7 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="4" t="s">
+      <c r="A148" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B148">
@@ -8976,7 +8926,7 @@
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="4" t="s">
+      <c r="A149" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B149">
@@ -8995,7 +8945,7 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="4" t="s">
+      <c r="A150" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B150">
@@ -9014,7 +8964,7 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="4" t="s">
+      <c r="A151" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B151">
@@ -9033,7 +8983,7 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="4" t="s">
+      <c r="A152" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B152">
@@ -9052,7 +9002,7 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
+      <c r="A153" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B153">
@@ -9071,7 +9021,7 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="4" t="s">
+      <c r="A154" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B154">
@@ -9090,7 +9040,7 @@
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+      <c r="A155" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B155">
@@ -9109,7 +9059,7 @@
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="4" t="s">
+      <c r="A156" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B156">
@@ -9128,7 +9078,7 @@
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B157">
@@ -9147,7 +9097,7 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="4" t="s">
+      <c r="A158" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B158">
@@ -9166,7 +9116,7 @@
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
+      <c r="A159" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B159">
@@ -9185,7 +9135,7 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
+      <c r="A160" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B160">
@@ -9204,7 +9154,7 @@
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
+      <c r="A161" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B161">
@@ -9223,7 +9173,7 @@
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" s="4" t="s">
+      <c r="A162" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B162">
@@ -9242,7 +9192,7 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" s="4" t="s">
+      <c r="A163" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B163">
@@ -9261,7 +9211,7 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
+      <c r="A164" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B164">
@@ -9280,7 +9230,7 @@
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
+      <c r="A165" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B165">
@@ -9299,7 +9249,7 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="4" t="s">
+      <c r="A166" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B166">
@@ -9318,7 +9268,7 @@
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="4" t="s">
+      <c r="A167" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B167">
@@ -9337,7 +9287,7 @@
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" s="4" t="s">
+      <c r="A168" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B168">
@@ -9356,7 +9306,7 @@
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
+      <c r="A169" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B169">
@@ -9375,7 +9325,7 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B170">
@@ -9394,7 +9344,7 @@
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
+      <c r="A171" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B171">
@@ -9413,7 +9363,7 @@
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="4" t="s">
+      <c r="A172" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B172">
@@ -9432,7 +9382,7 @@
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
+      <c r="A173" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B173">
@@ -9451,7 +9401,7 @@
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A174" s="4" t="s">
+      <c r="A174" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B174">
@@ -9470,7 +9420,7 @@
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175" s="4" t="s">
+      <c r="A175" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B175">
@@ -9489,7 +9439,7 @@
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" s="4" t="s">
+      <c r="A176" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B176">
@@ -9508,7 +9458,7 @@
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
+      <c r="A177" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B177">
@@ -9527,7 +9477,7 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" s="4" t="s">
+      <c r="A178" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B178">
@@ -9546,7 +9496,7 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" s="4" t="s">
+      <c r="A179" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B179">
@@ -9565,7 +9515,7 @@
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" s="4" t="s">
+      <c r="A180" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B180">
@@ -9584,7 +9534,7 @@
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B181">
@@ -9603,7 +9553,7 @@
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182" s="4" t="s">
+      <c r="A182" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B182">
@@ -9622,7 +9572,7 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" s="4" t="s">
+      <c r="A183" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B183">
@@ -9641,7 +9591,7 @@
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" s="4" t="s">
+      <c r="A184" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B184">
@@ -9660,7 +9610,7 @@
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A185" s="4" t="s">
+      <c r="A185" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B185">
@@ -9679,7 +9629,7 @@
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A186" s="4" t="s">
+      <c r="A186" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B186">
@@ -9698,7 +9648,7 @@
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A187" s="4" t="s">
+      <c r="A187" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B187">
@@ -9717,7 +9667,7 @@
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A188" s="4" t="s">
+      <c r="A188" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B188">
@@ -9736,7 +9686,7 @@
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A189" s="4" t="s">
+      <c r="A189" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B189">
@@ -9755,7 +9705,7 @@
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A190" s="4" t="s">
+      <c r="A190" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B190">
@@ -9774,7 +9724,7 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="4" t="s">
+      <c r="A191" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B191">
@@ -9793,7 +9743,7 @@
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A192" s="4" t="s">
+      <c r="A192" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B192">
@@ -9812,7 +9762,7 @@
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A193" s="4" t="s">
+      <c r="A193" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B193">
@@ -9831,7 +9781,7 @@
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A194" s="4" t="s">
+      <c r="A194" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B194">
@@ -9849,11 +9799,8 @@
         <v>-0.33752429332484185</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A195" s="2"/>
-    </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A196" s="5" t="s">
+      <c r="A196" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B196">
@@ -9872,7 +9819,7 @@
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A197" s="5" t="s">
+      <c r="A197" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B197">
@@ -9891,7 +9838,7 @@
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A198" s="5" t="s">
+      <c r="A198" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B198">
@@ -9910,7 +9857,7 @@
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A199" s="5" t="s">
+      <c r="A199" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B199">
@@ -9929,7 +9876,7 @@
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A200" s="5" t="s">
+      <c r="A200" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B200">
@@ -9948,7 +9895,7 @@
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A201" s="5" t="s">
+      <c r="A201" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B201">
@@ -9967,7 +9914,7 @@
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A202" s="5" t="s">
+      <c r="A202" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B202">
@@ -9986,7 +9933,7 @@
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A203" s="5" t="s">
+      <c r="A203" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B203">
@@ -10005,7 +9952,7 @@
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A204" s="5" t="s">
+      <c r="A204" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B204">
@@ -10024,7 +9971,7 @@
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A205" s="5" t="s">
+      <c r="A205" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B205">
@@ -10043,7 +9990,7 @@
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A206" s="5" t="s">
+      <c r="A206" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B206">
@@ -10062,7 +10009,7 @@
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" s="5" t="s">
+      <c r="A207" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B207">
@@ -10081,7 +10028,7 @@
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A208" s="5" t="s">
+      <c r="A208" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B208">
@@ -10100,7 +10047,7 @@
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209" s="5" t="s">
+      <c r="A209" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B209">
@@ -10119,7 +10066,7 @@
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" s="5" t="s">
+      <c r="A210" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B210">
@@ -10138,7 +10085,7 @@
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="5" t="s">
+      <c r="A211" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B211">
@@ -10157,7 +10104,7 @@
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" s="5" t="s">
+      <c r="A212" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B212">
@@ -10176,7 +10123,7 @@
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" s="5" t="s">
+      <c r="A213" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B213">
@@ -10195,7 +10142,7 @@
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" s="5" t="s">
+      <c r="A214" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B214">
@@ -10214,7 +10161,7 @@
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215" s="5" t="s">
+      <c r="A215" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B215">
@@ -10233,7 +10180,7 @@
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A216" s="5" t="s">
+      <c r="A216" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B216">
@@ -10252,7 +10199,7 @@
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217" s="5" t="s">
+      <c r="A217" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B217">
@@ -10271,7 +10218,7 @@
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218" s="5" t="s">
+      <c r="A218" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B218">
@@ -10290,7 +10237,7 @@
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A219" s="5" t="s">
+      <c r="A219" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B219">
@@ -10309,7 +10256,7 @@
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A220" s="5" t="s">
+      <c r="A220" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B220">
@@ -10328,7 +10275,7 @@
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A221" s="5" t="s">
+      <c r="A221" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B221">
@@ -10347,7 +10294,7 @@
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A222" s="5" t="s">
+      <c r="A222" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B222">
@@ -10366,7 +10313,7 @@
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A223" s="5" t="s">
+      <c r="A223" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B223">
@@ -10385,7 +10332,7 @@
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A224" s="5" t="s">
+      <c r="A224" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B224">
@@ -10404,7 +10351,7 @@
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A225" s="5" t="s">
+      <c r="A225" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B225">
@@ -10423,7 +10370,7 @@
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A226" s="5" t="s">
+      <c r="A226" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B226">
@@ -10442,7 +10389,7 @@
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A227" s="5" t="s">
+      <c r="A227" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B227">
@@ -10461,7 +10408,7 @@
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A228" s="5" t="s">
+      <c r="A228" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B228">
@@ -10480,7 +10427,7 @@
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A229" s="5" t="s">
+      <c r="A229" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B229">
@@ -10499,7 +10446,7 @@
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A230" s="5" t="s">
+      <c r="A230" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B230">
@@ -10518,7 +10465,7 @@
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A231" s="5" t="s">
+      <c r="A231" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B231">
@@ -10537,7 +10484,7 @@
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A232" s="5" t="s">
+      <c r="A232" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B232">
@@ -10556,7 +10503,7 @@
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A233" s="5" t="s">
+      <c r="A233" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B233">
@@ -10575,7 +10522,7 @@
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A234" s="5" t="s">
+      <c r="A234" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B234">
@@ -10594,7 +10541,7 @@
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A235" s="5" t="s">
+      <c r="A235" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B235">
@@ -10613,7 +10560,7 @@
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A236" s="5" t="s">
+      <c r="A236" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B236">
@@ -10632,7 +10579,7 @@
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A237" s="5" t="s">
+      <c r="A237" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B237">
@@ -10651,7 +10598,7 @@
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A238" s="5" t="s">
+      <c r="A238" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B238">
@@ -10670,7 +10617,7 @@
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A239" s="5" t="s">
+      <c r="A239" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B239">
@@ -10689,7 +10636,7 @@
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A240" s="5" t="s">
+      <c r="A240" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B240">
@@ -10708,7 +10655,7 @@
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A241" s="5" t="s">
+      <c r="A241" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B241">
@@ -10727,7 +10674,7 @@
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A242" s="5" t="s">
+      <c r="A242" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B242">
@@ -10746,7 +10693,7 @@
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A243" s="5" t="s">
+      <c r="A243" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B243">
@@ -10765,7 +10712,7 @@
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A244" s="5" t="s">
+      <c r="A244" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B244">
@@ -10784,7 +10731,7 @@
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A245" s="5" t="s">
+      <c r="A245" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B245">
@@ -10803,7 +10750,7 @@
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A246" s="5" t="s">
+      <c r="A246" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B246">
@@ -10822,7 +10769,7 @@
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A247" s="5" t="s">
+      <c r="A247" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B247">
@@ -10841,7 +10788,7 @@
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A248" s="5" t="s">
+      <c r="A248" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B248">
@@ -10860,7 +10807,7 @@
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A249" s="5" t="s">
+      <c r="A249" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B249">
@@ -10879,7 +10826,7 @@
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A250" s="5" t="s">
+      <c r="A250" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B250">
@@ -10898,7 +10845,7 @@
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A251" s="5" t="s">
+      <c r="A251" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B251">
@@ -10917,7 +10864,7 @@
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A252" s="5" t="s">
+      <c r="A252" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B252">
@@ -10936,7 +10883,7 @@
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A253" s="5" t="s">
+      <c r="A253" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B253">
@@ -10955,7 +10902,7 @@
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A254" s="5" t="s">
+      <c r="A254" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B254">
@@ -10974,7 +10921,7 @@
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A255" s="5" t="s">
+      <c r="A255" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B255">
@@ -10993,7 +10940,7 @@
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A256" s="5" t="s">
+      <c r="A256" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B256">
@@ -11012,7 +10959,7 @@
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A257" s="5" t="s">
+      <c r="A257" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B257">
@@ -11031,7 +10978,7 @@
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A258" s="5" t="s">
+      <c r="A258" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B258">
@@ -11050,7 +10997,7 @@
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A259" s="5" t="s">
+      <c r="A259" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B259">
@@ -11069,7 +11016,7 @@
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A260" s="5" t="s">
+      <c r="A260" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B260">
@@ -11088,7 +11035,7 @@
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A261" s="5" t="s">
+      <c r="A261" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B261">
@@ -11107,7 +11054,7 @@
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A262" s="5" t="s">
+      <c r="A262" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B262">
@@ -11126,7 +11073,7 @@
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A263" s="5" t="s">
+      <c r="A263" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B263">
@@ -11145,7 +11092,7 @@
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A264" s="5" t="s">
+      <c r="A264" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B264">
@@ -11164,7 +11111,7 @@
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A265" s="5" t="s">
+      <c r="A265" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B265">
@@ -11183,7 +11130,7 @@
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A266" s="5" t="s">
+      <c r="A266" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B266">
@@ -11202,7 +11149,7 @@
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A267" s="5" t="s">
+      <c r="A267" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B267">
@@ -11221,7 +11168,7 @@
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A268" s="5" t="s">
+      <c r="A268" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B268">
@@ -11240,7 +11187,7 @@
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A269" s="5" t="s">
+      <c r="A269" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B269">
@@ -11259,7 +11206,7 @@
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A270" s="5" t="s">
+      <c r="A270" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B270">
@@ -11278,7 +11225,7 @@
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A271" s="5" t="s">
+      <c r="A271" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B271">
@@ -11297,7 +11244,7 @@
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A272" s="5" t="s">
+      <c r="A272" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B272">
@@ -11316,7 +11263,7 @@
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A273" s="5" t="s">
+      <c r="A273" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B273">
@@ -11335,7 +11282,7 @@
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A274" s="5" t="s">
+      <c r="A274" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B274">
@@ -11354,7 +11301,7 @@
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A275" s="5" t="s">
+      <c r="A275" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B275">
@@ -11373,7 +11320,7 @@
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A276" s="5" t="s">
+      <c r="A276" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B276">
@@ -11392,7 +11339,7 @@
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A277" s="5" t="s">
+      <c r="A277" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B277">
@@ -11411,7 +11358,7 @@
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A278" s="5" t="s">
+      <c r="A278" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B278">
@@ -11430,7 +11377,7 @@
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A279" s="5" t="s">
+      <c r="A279" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B279">
@@ -11449,7 +11396,7 @@
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A280" s="5" t="s">
+      <c r="A280" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B280">
@@ -11468,7 +11415,7 @@
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A281" s="5" t="s">
+      <c r="A281" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B281">
@@ -11487,7 +11434,7 @@
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A282" s="5" t="s">
+      <c r="A282" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B282">
@@ -11506,7 +11453,7 @@
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A283" s="5" t="s">
+      <c r="A283" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B283">
@@ -11525,7 +11472,7 @@
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A284" s="5" t="s">
+      <c r="A284" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B284">
@@ -11544,7 +11491,7 @@
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A285" s="5" t="s">
+      <c r="A285" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B285">
@@ -11563,7 +11510,7 @@
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A286" s="5" t="s">
+      <c r="A286" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B286">
@@ -11582,7 +11529,7 @@
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" s="5" t="s">
+      <c r="A287" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B287">
@@ -11601,7 +11548,7 @@
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" s="5" t="s">
+      <c r="A288" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B288">
@@ -11620,7 +11567,7 @@
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" s="5" t="s">
+      <c r="A289" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B289">
@@ -11639,7 +11586,7 @@
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A290" s="5" t="s">
+      <c r="A290" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B290">
@@ -11658,7 +11605,7 @@
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A291" s="5" t="s">
+      <c r="A291" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B291">
@@ -11677,7 +11624,7 @@
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" s="5" t="s">
+      <c r="A292" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B292">
@@ -11696,7 +11643,7 @@
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A293" s="5" t="s">
+      <c r="A293" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B293">
@@ -11715,7 +11662,7 @@
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A294" s="5" t="s">
+      <c r="A294" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B294">
@@ -11734,7 +11681,7 @@
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A295" s="5" t="s">
+      <c r="A295" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B295">
@@ -11753,7 +11700,7 @@
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A296" s="5" t="s">
+      <c r="A296" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B296">
@@ -11772,7 +11719,7 @@
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A297" s="5" t="s">
+      <c r="A297" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B297">
@@ -11791,7 +11738,7 @@
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" s="5" t="s">
+      <c r="A298" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B298">
@@ -11810,7 +11757,7 @@
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A299" s="5" t="s">
+      <c r="A299" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B299">
@@ -11829,7 +11776,7 @@
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" s="5" t="s">
+      <c r="A300" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B300">
@@ -11848,7 +11795,7 @@
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A301" s="5" t="s">
+      <c r="A301" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B301">
@@ -11867,7 +11814,7 @@
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" s="5" t="s">
+      <c r="A302" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B302">
@@ -11886,7 +11833,7 @@
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A303" s="5" t="s">
+      <c r="A303" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B303">
@@ -11905,7 +11852,7 @@
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" s="5" t="s">
+      <c r="A304" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B304">
@@ -11924,7 +11871,7 @@
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A305" s="5" t="s">
+      <c r="A305" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B305">
@@ -11943,7 +11890,7 @@
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A306" s="5" t="s">
+      <c r="A306" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B306">
@@ -11962,7 +11909,7 @@
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A307" s="5" t="s">
+      <c r="A307" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B307">
@@ -11981,7 +11928,7 @@
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A308" s="5" t="s">
+      <c r="A308" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B308">
@@ -12000,7 +11947,7 @@
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A309" s="5" t="s">
+      <c r="A309" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B309">
@@ -12019,7 +11966,7 @@
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A310" s="5" t="s">
+      <c r="A310" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B310">
@@ -12038,7 +11985,7 @@
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A311" s="5" t="s">
+      <c r="A311" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B311">
@@ -12057,7 +12004,7 @@
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A312" s="5" t="s">
+      <c r="A312" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B312">
@@ -12076,7 +12023,7 @@
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A313" s="5" t="s">
+      <c r="A313" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B313">
@@ -12095,7 +12042,7 @@
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A314" s="5" t="s">
+      <c r="A314" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B314">
@@ -12114,7 +12061,7 @@
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A315" s="5" t="s">
+      <c r="A315" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B315">
@@ -12133,7 +12080,7 @@
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A316" s="5" t="s">
+      <c r="A316" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B316">
@@ -12152,7 +12099,7 @@
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A317" s="5" t="s">
+      <c r="A317" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B317">
@@ -12171,7 +12118,7 @@
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A318" s="5" t="s">
+      <c r="A318" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B318">
@@ -12190,7 +12137,7 @@
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A319" s="5" t="s">
+      <c r="A319" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B319">
@@ -12209,7 +12156,7 @@
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A320" s="5" t="s">
+      <c r="A320" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B320">
@@ -12228,7 +12175,7 @@
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A321" s="5" t="s">
+      <c r="A321" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B321">
@@ -12247,7 +12194,7 @@
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A322" s="5" t="s">
+      <c r="A322" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B322">
@@ -12266,7 +12213,7 @@
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A323" s="5" t="s">
+      <c r="A323" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B323">
@@ -12285,7 +12232,7 @@
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A324" s="5" t="s">
+      <c r="A324" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B324">
@@ -12304,7 +12251,7 @@
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A325" s="5" t="s">
+      <c r="A325" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B325">
@@ -12323,7 +12270,7 @@
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A326" s="5" t="s">
+      <c r="A326" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B326">
@@ -12342,7 +12289,7 @@
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A327" s="5" t="s">
+      <c r="A327" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B327">
@@ -12361,7 +12308,7 @@
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A328" s="5" t="s">
+      <c r="A328" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B328">
@@ -12380,7 +12327,7 @@
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A329" s="5" t="s">
+      <c r="A329" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B329">
@@ -12399,7 +12346,7 @@
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A330" s="5" t="s">
+      <c r="A330" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B330">
@@ -12418,7 +12365,7 @@
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A331" s="5" t="s">
+      <c r="A331" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B331">
@@ -12437,7 +12384,7 @@
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A332" s="5" t="s">
+      <c r="A332" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B332">
@@ -12456,7 +12403,7 @@
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A333" s="5" t="s">
+      <c r="A333" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B333">
@@ -12475,7 +12422,7 @@
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A334" s="5" t="s">
+      <c r="A334" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B334">
@@ -12494,7 +12441,7 @@
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A335" s="5" t="s">
+      <c r="A335" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B335">
@@ -12513,7 +12460,7 @@
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A336" s="5" t="s">
+      <c r="A336" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B336">
@@ -12532,7 +12479,7 @@
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A337" s="5" t="s">
+      <c r="A337" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B337">
@@ -12551,7 +12498,7 @@
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A338" s="5" t="s">
+      <c r="A338" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B338">
@@ -12570,7 +12517,7 @@
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A339" s="5" t="s">
+      <c r="A339" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B339">
@@ -12589,7 +12536,7 @@
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A340" s="5" t="s">
+      <c r="A340" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B340">
@@ -12608,7 +12555,7 @@
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A341" s="5" t="s">
+      <c r="A341" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B341">
@@ -12627,7 +12574,7 @@
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A342" s="5" t="s">
+      <c r="A342" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B342">
@@ -12646,7 +12593,7 @@
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A343" s="5" t="s">
+      <c r="A343" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B343">
@@ -12665,7 +12612,7 @@
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A344" s="5" t="s">
+      <c r="A344" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B344">
@@ -12684,7 +12631,7 @@
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A345" s="5" t="s">
+      <c r="A345" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B345">
@@ -12703,7 +12650,7 @@
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A346" s="5" t="s">
+      <c r="A346" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B346">
@@ -12722,7 +12669,7 @@
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A347" s="5" t="s">
+      <c r="A347" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B347">
@@ -12741,7 +12688,7 @@
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A348" s="5" t="s">
+      <c r="A348" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B348">
@@ -12760,7 +12707,7 @@
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A349" s="5" t="s">
+      <c r="A349" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B349">
@@ -12779,7 +12726,7 @@
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A350" s="5" t="s">
+      <c r="A350" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B350">
@@ -12815,21 +12762,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3">
@@ -12848,7 +12795,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -12867,7 +12814,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5">
@@ -12886,7 +12833,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
@@ -12905,7 +12852,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -12924,7 +12871,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -12943,7 +12890,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B9">
@@ -12962,7 +12909,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B10">
@@ -12981,7 +12928,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B11">
@@ -13000,7 +12947,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B12">
@@ -13019,7 +12966,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B13">
@@ -13038,7 +12985,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B14">
@@ -13057,7 +13004,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B15">
@@ -13076,7 +13023,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B16">
@@ -13095,7 +13042,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B17">
@@ -13114,7 +13061,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B18">
@@ -13133,7 +13080,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B19">
@@ -13152,7 +13099,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B20">
@@ -13171,7 +13118,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B21">
@@ -13190,7 +13137,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B22">
@@ -13209,7 +13156,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B23">
@@ -13228,7 +13175,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B24">
@@ -13247,7 +13194,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B25">
@@ -13266,7 +13213,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B26">
@@ -13285,7 +13232,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B27">
@@ -13304,7 +13251,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B28">
@@ -13323,7 +13270,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B29">
@@ -13342,7 +13289,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B30">
@@ -13361,7 +13308,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B31">
@@ -13380,7 +13327,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B32">
@@ -13399,7 +13346,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B33">
@@ -13418,7 +13365,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B34">
@@ -13437,7 +13384,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B35">
@@ -13456,7 +13403,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B36">
@@ -13475,7 +13422,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B37">
@@ -13494,7 +13441,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B38">
@@ -13513,7 +13460,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B39">
@@ -13532,7 +13479,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B40">
@@ -13551,7 +13498,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B41">
@@ -13570,7 +13517,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B42">
@@ -13589,7 +13536,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B43">
@@ -13608,7 +13555,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B44">
@@ -13627,7 +13574,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B45">
@@ -13646,7 +13593,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B46">
@@ -13665,7 +13612,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B47">
@@ -13684,7 +13631,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B48">
@@ -13703,7 +13650,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B49">
@@ -13722,7 +13669,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B51">
@@ -13741,7 +13688,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B52">
@@ -13760,7 +13707,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B53">
@@ -13779,7 +13726,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B54">
@@ -13798,7 +13745,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B55">
@@ -13817,7 +13764,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B56">
@@ -13836,7 +13783,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B57">
@@ -13855,7 +13802,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B58">
@@ -13874,7 +13821,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B59">
@@ -13893,7 +13840,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B60">
@@ -13912,7 +13859,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B61">
@@ -13931,7 +13878,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B62">
@@ -13950,7 +13897,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B63">
@@ -13969,7 +13916,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B64">
@@ -13988,7 +13935,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B65">
@@ -14007,7 +13954,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B66">
@@ -14026,7 +13973,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B67">
@@ -14045,7 +13992,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B68">
@@ -14064,7 +14011,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B69">
@@ -14083,7 +14030,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B70">
@@ -14102,7 +14049,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B71">
@@ -14121,7 +14068,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B72">
@@ -14140,7 +14087,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B73">
@@ -14159,7 +14106,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B74">
@@ -14178,7 +14125,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B75">
@@ -14197,7 +14144,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B76">
@@ -14216,7 +14163,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B77">
@@ -14254,21 +14201,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1">
@@ -14287,7 +14234,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -14297,16 +14244,16 @@
         <v>0.94283751570017804</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D7" si="0">LOG(B4)</f>
+        <f t="shared" ref="D4:D6" si="0">LOG(B4)</f>
         <v>-2.4845841908073916</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E7" si="1">LOG(C4)</f>
+        <f t="shared" ref="E4:E6" si="1">LOG(C4)</f>
         <v>-2.5563145136449961E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1">
@@ -14325,7 +14272,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1">
@@ -14344,7 +14291,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">

</xml_diff>